<commit_message>
Firbase implementation of Nabsim - first commit
</commit_message>
<xml_diff>
--- a/kieranJan21.xlsx
+++ b/kieranJan21.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="97">
   <si>
     <t>Sarah Bowman</t>
   </si>
@@ -455,6 +456,21 @@
   </si>
   <si>
     <t>not significant</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>Happy</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Unhappy</t>
   </si>
 </sst>
 </file>
@@ -776,20 +792,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="38.3046875" customWidth="1"/>
-    <col min="2" max="2" width="17.4609375" customWidth="1"/>
-    <col min="3" max="3" width="17.765625" customWidth="1"/>
+    <col min="2" max="2" width="11.53515625" customWidth="1"/>
+    <col min="3" max="3" width="1.3828125" customWidth="1"/>
     <col min="4" max="4" width="11.53515625" customWidth="1"/>
-    <col min="5" max="5" width="50.07421875" customWidth="1"/>
-    <col min="6" max="6" width="32.69140625" customWidth="1"/>
+    <col min="5" max="5" width="40.23046875" customWidth="1"/>
+    <col min="6" max="6" width="7.23046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.84375" customWidth="1"/>
+    <col min="8" max="8" width="1.61328125" customWidth="1"/>
+    <col min="9" max="9" width="15.84375" customWidth="1"/>
+    <col min="10" max="10" width="9.23046875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
@@ -1059,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
@@ -1257,7 +1277,7 @@
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
         <v>29</v>
@@ -2118,4 +2138,51 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1">
+        <f>B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <f>B1-B2</f>
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>